<commit_message>
Copy Files From Source Repo (2025-01-31 21:07)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
+++ b/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
@@ -46,7 +46,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Tanggal</t>
+      <t>Publikasi</t>
     </r>
   </si>
   <si>
@@ -432,7 +432,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F14" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="1" headerRowBorderDxfId="2">
   <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Tanggal" dataDxfId="0"/>
+    <tableColumn id="1" name="Publikasi" dataDxfId="0"/>
     <tableColumn id="2" name="Total Penjualan Chai (unit)"/>
     <tableColumn id="3" name="Penjualan Artisanal Chai (unit)"/>
     <tableColumn id="4" name="Premade Chai Sales (unit)"/>

</xml_diff>